<commit_message>
Fix export form definition
Instead of cast votes, we really need the invalid and empty votes.
</commit_message>
<xml_diff>
--- a/src/onegov.election_day/docs/vorlage.xlsx
+++ b/src/onegov.election_day/docs/vorlage.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="8">
   <si>
     <t>Bezirk</t>
   </si>
@@ -32,7 +32,10 @@
     <t>Stimmberechtigte</t>
   </si>
   <si>
-    <t>Eingelegte Stimmzettel</t>
+    <t>Leere Stimmzettel</t>
+  </si>
+  <si>
+    <t>Ungültige Stimmzettel</t>
   </si>
 </sst>
 </file>
@@ -42,7 +45,7 @@
   <numFmts count="1">
     <numFmt numFmtId="0" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color indexed="8"/>
@@ -54,12 +57,17 @@
       <name val="Helvetica"/>
     </font>
     <font>
-      <sz val="10"/>
+      <sz val="12"/>
       <color indexed="8"/>
       <name val="Verdana"/>
     </font>
     <font>
-      <sz val="13"/>
+      <sz val="15"/>
+      <color indexed="8"/>
+      <name val="Verdana"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color indexed="8"/>
       <name val="Verdana"/>
     </font>
@@ -72,7 +80,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -95,21 +103,135 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="9"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="9"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="9"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="9"/>
+      </right>
+      <top style="thin">
+        <color indexed="9"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="9"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="9"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="9"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="9"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="9"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="9"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="9"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom"/>
+    <xf numFmtId="0" fontId="2" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1360,11 +1482,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6" defaultRowHeight="13" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="6.625" defaultRowHeight="13" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="1" max="1" width="6" style="1" customWidth="1"/>
     <col min="2" max="2" width="6" style="1" customWidth="1"/>
@@ -1373,7 +1495,8 @@
     <col min="5" max="5" width="6" style="1" customWidth="1"/>
     <col min="6" max="6" width="6" style="1" customWidth="1"/>
     <col min="7" max="7" width="6" style="1" customWidth="1"/>
-    <col min="8" max="256" width="6" style="1" customWidth="1"/>
+    <col min="8" max="8" width="6" style="1" customWidth="1"/>
+    <col min="9" max="256" width="6.625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="17" customHeight="1">
@@ -1398,6 +1521,99 @@
       <c r="G1" t="s" s="2">
         <v>6</v>
       </c>
+      <c r="H1" t="s" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" ht="20" customHeight="1">
+      <c r="A2" s="3"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="5"/>
+    </row>
+    <row r="3" ht="20" customHeight="1">
+      <c r="A3" s="6"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="8"/>
+    </row>
+    <row r="4" ht="20" customHeight="1">
+      <c r="A4" s="6"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="8"/>
+    </row>
+    <row r="5" ht="20" customHeight="1">
+      <c r="A5" s="6"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="8"/>
+    </row>
+    <row r="6" ht="20" customHeight="1">
+      <c r="A6" s="6"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="8"/>
+    </row>
+    <row r="7" ht="20" customHeight="1">
+      <c r="A7" s="6"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="8"/>
+    </row>
+    <row r="8" ht="20" customHeight="1">
+      <c r="A8" s="6"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="8"/>
+    </row>
+    <row r="9" ht="20" customHeight="1">
+      <c r="A9" s="6"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="8"/>
+    </row>
+    <row r="10" ht="20" customHeight="1">
+      <c r="A10" s="9"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="10"/>
+      <c r="H10" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>